<commit_message>
updated results excel and json
</commit_message>
<xml_diff>
--- a/static/excel/results.xlsx
+++ b/static/excel/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkcsh\dev\iiot2025.github.io\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88E5D1B-D7D7-4778-89A2-9C59B6C6A6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C6C7E1-C278-4FB8-A6BF-5C4FB3BAAC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{51F6ACA9-91B5-41CE-84B3-13292AFF13FC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="110">
   <si>
     <t>Team</t>
   </si>
@@ -355,6 +355,15 @@
   </si>
   <si>
     <t>Kodsport Sverige</t>
+  </si>
+  <si>
+    <t>honorary gold</t>
+  </si>
+  <si>
+    <t>honorary silver</t>
+  </si>
+  <si>
+    <t>honorary bronze</t>
   </si>
 </sst>
 </file>
@@ -430,7 +439,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1469,13 +1499,13 @@
     <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <conditionalFormatting sqref="A1:N1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$B1="bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$B1="silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$B1="gold"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1488,9 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C56E6AD-BB8B-4DF2-A4D5-F54BE7F053B5}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1553,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>93</v>
@@ -1597,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>95</v>
@@ -1641,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>97</v>
@@ -1685,7 +1713,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>99</v>
@@ -1729,7 +1757,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C6" s="1">
         <v>42</v>
@@ -1893,14 +1921,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:N1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$B1="bronze"</formula>
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$B1="honorary bronze"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$B1="silver"</formula>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$B1="honorary silver"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$B1="gold"</formula>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$B1="honorary gold"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>